<commit_message>
created excel with request explained
</commit_message>
<xml_diff>
--- a/api_requests.xlsx
+++ b/api_requests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\modules\user-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDE71EA-13FD-448F-8F63-18FC56C49EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46AD453-17D5-483F-9672-282D884817B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19185" yWindow="5010" windowWidth="19185" windowHeight="10575" xr2:uid="{6EE3E343-B8B8-4D2F-97B6-15ED9E96716B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EE3E343-B8B8-4D2F-97B6-15ED9E96716B}"/>
   </bookViews>
   <sheets>
     <sheet name="usermanager" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Usermanager API Funktionen:</t>
   </si>
@@ -77,9 +77,6 @@
     <t>201 (=user was created)</t>
   </si>
   <si>
-    <t>success | status 200</t>
-  </si>
-  <si>
     <t>status: 400</t>
   </si>
   <si>
@@ -87,10 +84,6 @@
   </si>
   <si>
     <t>status: 500</t>
-  </si>
-  <si>
-    <t>wrong username/sessionKey
-or session lastAction was to long ago)</t>
   </si>
   <si>
     <t>missing data/not valid data</t>
@@ -108,16 +101,158 @@
     <t>oldUsername
 newUsername
 sessionKey</t>
+  </si>
+  <si>
+    <t>wrong username/sessionKey
+or session lastAction was to long ago</t>
+  </si>
+  <si>
+    <t>success | status 200/201</t>
+  </si>
+  <si>
+    <t>201 (=Username was changed)</t>
+  </si>
+  <si>
+    <t>change Email</t>
+  </si>
+  <si>
+    <t>username
+newEmail
+password
+sessionKey</t>
+  </si>
+  <si>
+    <t>missing data/not valid data/username exists</t>
+  </si>
+  <si>
+    <t>missing data/not valid data/email exists</t>
+  </si>
+  <si>
+    <t>201 (=Email was changed)</t>
+  </si>
+  <si>
+    <t>/userManager/change/password</t>
+  </si>
+  <si>
+    <t>/userManager/change/username</t>
+  </si>
+  <si>
+    <t>/userManager/change/email</t>
+  </si>
+  <si>
+    <t>change ProfilePicture</t>
+  </si>
+  <si>
+    <t>not Implemented</t>
+  </si>
+  <si>
+    <t>request type</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>get UserData by username</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>/userManager/get/UserData_by_username/&lt;username&gt;</t>
+  </si>
+  <si>
+    <t>missing data/username not existing/</t>
+  </si>
+  <si>
+    <t>signIn user</t>
+  </si>
+  <si>
+    <t>username
+password</t>
+  </si>
+  <si>
+    <t>username or password wrong</t>
+  </si>
+  <si>
+    <t>missing data</t>
+  </si>
+  <si>
+    <t>/userManager/SignIn_User</t>
+  </si>
+  <si>
+    <t>signOut user</t>
+  </si>
+  <si>
+    <t>update Session</t>
+  </si>
+  <si>
+    <t>get LogginState</t>
+  </si>
+  <si>
+    <t>new SessionKey</t>
+  </si>
+  <si>
+    <t>/userManager/new_sessionKey</t>
+  </si>
+  <si>
+    <t>/userManager/get_LogginState</t>
+  </si>
+  <si>
+    <t>/userManager/updateSession</t>
+  </si>
+  <si>
+    <t>/userManager/SignOut_User</t>
+  </si>
+  <si>
+    <t>username
+sessionKey</t>
+  </si>
+  <si>
+    <t>status: 201 (=user session was Deleted, 
+user is no longer signed In)</t>
+  </si>
+  <si>
+    <t>status: 201 (=user session was updated)</t>
+  </si>
+  <si>
+    <t>status: 201 (=signIn successful sessionKey was returned),
+sessionKey: ""</t>
+  </si>
+  <si>
+    <t>status: 201 (=new sessionKey was created 
+and new SessionKey got returned)
+newSessionKey: ""</t>
+  </si>
+  <si>
+    <t>status: 200 (=request successful data was returned),
+data: username: ""/email: ""/
+profilePicture: ""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: 200 (=user is signed in Session isn't 
+expired) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,13 +267,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,11 +307,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -185,6 +320,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FF003399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -493,179 +634,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75132D7E-425B-48D2-9E98-34FD18A0387E}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -673,8 +967,9 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -682,8 +977,9 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -691,8 +987,9 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -700,8 +997,9 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -709,8 +1007,10 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>